<commit_message>
update to schematic but something on layout is broken
</commit_message>
<xml_diff>
--- a/Chicker/POWER_BOARD_BOM_BASIC_TESTBOARD.xlsx
+++ b/Chicker/POWER_BOARD_BOM_BASIC_TESTBOARD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The Bots\Electrical\PowerBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The_Bots\Electrical\Chicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E962606-B303-4983-8A86-39C560A3E3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA56D977-78F5-4E14-A67B-7CE1A18F07AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5112" yWindow="17172" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="340">
   <si>
     <t>Reference</t>
   </si>
@@ -1122,6 +1122,9 @@
   </si>
   <si>
     <t>bots:D_SOD-323_HandSoldering</t>
+  </si>
+  <si>
+    <t>discount</t>
   </si>
 </sst>
 </file>
@@ -1461,13 +1464,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1633,19 +1636,23 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2044,8 +2051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K43" zoomScale="101" workbookViewId="0">
-      <selection activeCell="R56" sqref="R56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="101" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2138,73 +2145,76 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="6">
         <v>1.4710000000000001</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="6">
         <v>1.0630500000000001</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="6">
         <v>2</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="6">
         <f>L2-K2</f>
         <v>2</v>
       </c>
-      <c r="O2">
+      <c r="N2" s="6">
+        <v>3</v>
+      </c>
+      <c r="O2" s="6">
+        <f>IF(M2-N2&lt;0,0, M2-N2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="6">
+        <f>IF(W2="DIGIKEY",O2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6">
+        <f>IFN2*8</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="6">
         <f>M2*5</f>
         <v>10</v>
       </c>
-      <c r="P2">
-        <f>IF(W2="DIGIKEY",O2,0)</f>
-        <v>10</v>
-      </c>
-      <c r="Q2">
-        <f>IFN2*8</f>
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <f>M2*5</f>
-        <v>10</v>
-      </c>
-      <c r="S2">
+      <c r="S2" s="6">
         <f t="shared" ref="S2:S65" si="0">IF(O2&gt;10,H2*O2,G2*O2)</f>
-        <v>19.7</v>
-      </c>
-      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6">
         <f t="shared" ref="T2:T65" si="1">IF(ISBLANK(D2),"EMPTY",(I2*R2+IF(D2="yes",4.04,0)))</f>
         <v>14.670500000000001</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="6">
         <f t="shared" ref="V2:V33" si="2">IF(T2="EMPTY",S2,IF(J2="Bottom",S2,IF(U2="DIGIKEY",S2,IF(U2="JLC",T2,IF(T2&lt;S2+0.2,T2,S2)))))</f>
-        <v>19.7</v>
-      </c>
-      <c r="W2" t="str">
+        <v>0</v>
+      </c>
+      <c r="W2" s="6" t="str">
         <f t="shared" ref="W2:W33" si="3">IF(T2="EMPTY","DIGIKEY",IF(J2="Bottom","DIGIKEY",IF(U2="DIGIKEY",U2,IF(U2="JLC",U2,IF(T2&lt;S2+0.2,"JLC","DIGIKEY")))))</f>
         <v>DIGIKEY</v>
       </c>
@@ -2245,8 +2255,8 @@
         <v>3</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O66" si="5">M3*5</f>
-        <v>15</v>
+        <f t="shared" ref="O3:O66" si="5">IF(M3-N3&lt;0,0, M3-N3)</f>
+        <v>3</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P66" si="6">IF(W3="DIGIKEY",O3,0)</f>
@@ -2262,7 +2272,7 @@
       </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>5.07</v>
+        <v>1.53</v>
       </c>
       <c r="T3">
         <f t="shared" si="1"/>
@@ -2277,71 +2287,71 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="6">
         <v>7.53</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="6">
         <v>2</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="6">
         <v>8</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="6">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
         <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="6">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="6">
         <f t="shared" si="0"/>
-        <v>87.6</v>
-      </c>
-      <c r="T4" t="str">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="6">
         <f t="shared" si="2"/>
-        <v>87.6</v>
-      </c>
-      <c r="W4" t="str">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="X4" s="6" t="s">
         <v>331</v>
       </c>
     </row>
@@ -2382,11 +2392,11 @@
       </c>
       <c r="O5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q5">
         <f t="shared" si="7"/>
@@ -2398,22 +2408,19 @@
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>0.70000000000000007</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="T5">
         <f t="shared" si="1"/>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="U5" t="s">
-        <v>286</v>
-      </c>
       <c r="V5">
         <f t="shared" si="2"/>
-        <v>0.70000000000000007</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="3"/>
-        <v>DIGIKEY</v>
+        <v>JLC</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -2453,7 +2460,7 @@
       </c>
       <c r="O6">
         <f t="shared" si="5"/>
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="P6">
         <f t="shared" si="6"/>
@@ -2469,7 +2476,7 @@
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>2.4449999999999998</v>
+        <v>0.48899999999999993</v>
       </c>
       <c r="T6">
         <f t="shared" si="1"/>
@@ -2484,76 +2491,76 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="6">
         <v>0.156</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="6">
         <v>3.9600000000000003E-2</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="6">
         <v>2</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="6">
         <v>2</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="6">
         <f t="shared" si="1"/>
         <v>4.04</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W7" t="str">
+      <c r="W7" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
@@ -2595,7 +2602,7 @@
       </c>
       <c r="O8">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="P8">
         <f t="shared" si="6"/>
@@ -2611,7 +2618,7 @@
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>6.34</v>
+        <v>1.92</v>
       </c>
       <c r="T8">
         <f t="shared" si="1"/>
@@ -2663,7 +2670,7 @@
       </c>
       <c r="O9">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="P9">
         <f t="shared" si="6"/>
@@ -2679,7 +2686,7 @@
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>1.98</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="T9">
         <f t="shared" si="1"/>
@@ -2694,75 +2701,75 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="6">
         <v>4.7E-2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="6">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="6">
         <v>2</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="6">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="P10" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="6">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="6">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="6">
         <f t="shared" si="0"/>
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="T10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="T10" s="6">
         <f t="shared" si="1"/>
         <v>2.7000000000000003E-2</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="6">
         <f t="shared" si="2"/>
         <v>2.7000000000000003E-2</v>
       </c>
-      <c r="W10" t="str">
+      <c r="W10" s="6" t="str">
         <f t="shared" si="3"/>
         <v>JLC</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2802,11 +2809,11 @@
       </c>
       <c r="O11">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P11">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q11">
         <f t="shared" si="7"/>
@@ -2818,7 +2825,7 @@
       </c>
       <c r="S11">
         <f t="shared" si="0"/>
-        <v>0.70000000000000007</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="T11">
         <f t="shared" si="1"/>
@@ -2826,77 +2833,80 @@
       </c>
       <c r="V11">
         <f t="shared" si="2"/>
-        <v>0.70000000000000007</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="8">
         <v>0.61</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="6">
         <v>0.40799999999999997</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="6">
         <v>0.36230000000000001</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
+      <c r="L12" s="6">
+        <v>1</v>
+      </c>
+      <c r="M12" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O12">
+      <c r="N12" s="6">
+        <v>5</v>
+      </c>
+      <c r="O12" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="P12" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="6">
         <f t="shared" si="0"/>
-        <v>3.05</v>
-      </c>
-      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="T12" s="6">
         <f t="shared" si="1"/>
         <v>5.8514999999999997</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="6">
         <f t="shared" si="2"/>
-        <v>3.05</v>
-      </c>
-      <c r="W12" t="str">
+        <v>0</v>
+      </c>
+      <c r="W12" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
@@ -2938,7 +2948,7 @@
       </c>
       <c r="O13">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P13">
         <f t="shared" si="6"/>
@@ -2954,7 +2964,7 @@
       </c>
       <c r="S13">
         <f t="shared" si="0"/>
-        <v>1.4000000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="T13">
         <f t="shared" si="1"/>
@@ -2969,76 +2979,76 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="8">
         <v>0.62</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="6">
         <v>0.53400000000000003</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="6">
         <v>7.5300000000000006E-2</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="6">
         <v>2</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="6">
         <v>2</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="6">
         <f t="shared" si="1"/>
         <v>4.04</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W14" t="str">
+      <c r="W14" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
@@ -3117,70 +3127,70 @@
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="6">
         <v>0.53</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="6">
         <v>0.1038</v>
       </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
+      <c r="L16" s="6">
+        <v>1</v>
+      </c>
+      <c r="M16" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="P16" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="6">
         <f t="shared" si="0"/>
-        <v>3.4000000000000004</v>
-      </c>
-      <c r="T16">
+        <v>0.68</v>
+      </c>
+      <c r="T16" s="6">
         <f t="shared" si="1"/>
         <v>4.5590000000000002</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="6">
         <f t="shared" si="2"/>
-        <v>3.4000000000000004</v>
-      </c>
-      <c r="W16" t="str">
+        <v>0.68</v>
+      </c>
+      <c r="W16" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
@@ -3204,7 +3214,7 @@
       <c r="F17" t="s">
         <v>237</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="3">
         <v>0.39</v>
       </c>
       <c r="H17">
@@ -3222,7 +3232,7 @@
       </c>
       <c r="O17">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P17">
         <f t="shared" si="6"/>
@@ -3238,7 +3248,7 @@
       </c>
       <c r="S17">
         <f t="shared" si="0"/>
-        <v>1.9500000000000002</v>
+        <v>0.39</v>
       </c>
       <c r="T17">
         <f t="shared" si="1"/>
@@ -3253,73 +3263,73 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="6">
         <v>0.47399999999999998</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="6">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
+      <c r="L18" s="6">
+        <v>1</v>
+      </c>
+      <c r="M18" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="P18" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="6">
         <f t="shared" si="0"/>
-        <v>3.4000000000000004</v>
-      </c>
-      <c r="T18">
+        <v>0.68</v>
+      </c>
+      <c r="T18" s="6">
         <f t="shared" si="1"/>
         <v>4.4565000000000001</v>
       </c>
-      <c r="U18" t="s">
+      <c r="U18" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="6">
         <f t="shared" si="2"/>
         <v>4.4565000000000001</v>
       </c>
-      <c r="W18" t="str">
+      <c r="W18" s="6" t="str">
         <f t="shared" si="3"/>
         <v>JLC</v>
       </c>
@@ -3343,7 +3353,7 @@
       <c r="F19" t="s">
         <v>235</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="3">
         <v>0.39</v>
       </c>
       <c r="H19">
@@ -3361,7 +3371,7 @@
       </c>
       <c r="O19">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="P19">
         <f t="shared" si="6"/>
@@ -3377,7 +3387,7 @@
       </c>
       <c r="S19">
         <f t="shared" si="0"/>
-        <v>3.2399999999999998</v>
+        <v>1.17</v>
       </c>
       <c r="T19">
         <f t="shared" si="1"/>
@@ -3411,7 +3421,7 @@
       <c r="F20" t="s">
         <v>234</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="3">
         <v>0.39</v>
       </c>
       <c r="H20">
@@ -3429,7 +3439,7 @@
       </c>
       <c r="O20">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P20">
         <f t="shared" si="6"/>
@@ -3445,7 +3455,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="0"/>
-        <v>1.9500000000000002</v>
+        <v>0.39</v>
       </c>
       <c r="T20">
         <f t="shared" si="1"/>
@@ -3479,7 +3489,7 @@
       <c r="F21" t="s">
         <v>233</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="3">
         <v>0.39</v>
       </c>
       <c r="H21">
@@ -3497,7 +3507,7 @@
       </c>
       <c r="O21">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P21">
         <f t="shared" si="6"/>
@@ -3513,7 +3523,7 @@
       </c>
       <c r="S21">
         <f t="shared" si="0"/>
-        <v>3.9000000000000004</v>
+        <v>0.78</v>
       </c>
       <c r="T21">
         <f t="shared" si="1"/>
@@ -3528,212 +3538,212 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="6">
         <v>0.436</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="6">
         <v>0.63</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="M22">
+      <c r="L22" s="6">
+        <v>1</v>
+      </c>
+      <c r="M22" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="P22" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="6">
         <f t="shared" si="0"/>
-        <v>3.05</v>
-      </c>
-      <c r="T22" t="str">
+        <v>0.61</v>
+      </c>
+      <c r="T22" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V22">
+      <c r="V22" s="6">
         <f t="shared" si="2"/>
-        <v>3.05</v>
-      </c>
-      <c r="W22" t="str">
+        <v>0.61</v>
+      </c>
+      <c r="W22" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="8">
         <v>0.17</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="6">
         <v>0.122</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="6">
         <v>0.1038</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="M23">
+      <c r="L23" s="6">
+        <v>1</v>
+      </c>
+      <c r="M23" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="P23" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="6">
         <f t="shared" si="0"/>
-        <v>0.85000000000000009</v>
-      </c>
-      <c r="T23">
+        <v>0.17</v>
+      </c>
+      <c r="T23" s="6">
         <f t="shared" si="1"/>
         <v>0.51900000000000002</v>
       </c>
-      <c r="V23">
+      <c r="V23" s="6">
         <f t="shared" si="2"/>
-        <v>0.85000000000000009</v>
-      </c>
-      <c r="W23" t="str">
+        <v>0.17</v>
+      </c>
+      <c r="W23" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="8">
         <v>1.54</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="6">
         <v>1.4</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="6">
         <v>9.9199999999999997E-2</v>
       </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-      <c r="M24">
+      <c r="L24" s="6">
+        <v>1</v>
+      </c>
+      <c r="M24" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="P24" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="6">
         <f t="shared" si="0"/>
-        <v>7.7</v>
-      </c>
-      <c r="T24">
+        <v>1.54</v>
+      </c>
+      <c r="T24" s="6">
         <f t="shared" si="1"/>
         <v>4.5359999999999996</v>
       </c>
-      <c r="U24" t="s">
+      <c r="U24" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="6">
         <f t="shared" si="2"/>
-        <v>7.7</v>
-      </c>
-      <c r="W24" t="str">
+        <v>1.54</v>
+      </c>
+      <c r="W24" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
@@ -3803,64 +3813,64 @@
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="6">
         <v>1.3140000000000001</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="6">
         <v>1.61</v>
       </c>
-      <c r="L26">
-        <v>1</v>
-      </c>
-      <c r="M26">
+      <c r="L26" s="6">
+        <v>1</v>
+      </c>
+      <c r="M26" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="P26" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="6">
         <f t="shared" si="0"/>
-        <v>7.8000000000000007</v>
-      </c>
-      <c r="T26" t="str">
+        <v>1.56</v>
+      </c>
+      <c r="T26" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V26">
+      <c r="V26" s="6">
         <f t="shared" si="2"/>
-        <v>7.8000000000000007</v>
-      </c>
-      <c r="W26" t="str">
+        <v>1.56</v>
+      </c>
+      <c r="W26" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
@@ -4011,7 +4021,7 @@
       <c r="F29" t="s">
         <v>258</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="3">
         <v>0.5</v>
       </c>
       <c r="H29">
@@ -4029,7 +4039,7 @@
       </c>
       <c r="O29">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P29">
         <f t="shared" si="6"/>
@@ -4045,7 +4055,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T29">
         <f t="shared" si="1"/>
@@ -4060,283 +4070,289 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="30" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="6">
         <v>1.17</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="6">
         <v>0.46500000000000002</v>
       </c>
-      <c r="L30">
-        <v>1</v>
-      </c>
-      <c r="M30">
+      <c r="L30" s="6">
+        <v>1</v>
+      </c>
+      <c r="M30" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O30">
+      <c r="N30" s="6">
+        <v>10</v>
+      </c>
+      <c r="O30" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="P30" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R30">
+      <c r="R30" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="6">
         <f t="shared" si="0"/>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="T30" s="6">
         <f t="shared" si="1"/>
         <v>6.3650000000000002</v>
       </c>
-      <c r="U30" t="s">
+      <c r="U30" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="V30">
+      <c r="V30" s="6">
         <f t="shared" si="2"/>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="W30" t="str">
+        <v>0</v>
+      </c>
+      <c r="W30" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="6">
         <v>6.22</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="6">
         <v>4.0393999999999997</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="6">
         <v>2</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="6">
         <v>2</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N31">
-        <v>8</v>
-      </c>
-      <c r="O31">
+      <c r="N31" s="6">
+        <v>15</v>
+      </c>
+      <c r="O31" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="R31">
+      <c r="R31" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S31">
+      <c r="S31" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T31">
+      <c r="T31" s="6">
         <f t="shared" si="1"/>
         <v>4.04</v>
       </c>
-      <c r="U31" t="s">
+      <c r="U31" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="V31">
+      <c r="V31" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W31" t="str">
+      <c r="W31" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="X31" t="s">
+      <c r="X31" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Y31" s="6" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="32" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="6">
         <v>0.65</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L32">
-        <v>1</v>
-      </c>
-      <c r="M32">
+      <c r="L32" s="6">
+        <v>1</v>
+      </c>
+      <c r="M32" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="P32" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S32">
+      <c r="S32" s="6">
         <f t="shared" si="0"/>
-        <v>3.25</v>
-      </c>
-      <c r="T32" t="str">
+        <v>0.65</v>
+      </c>
+      <c r="T32" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V32">
+      <c r="V32" s="6">
         <f t="shared" si="2"/>
-        <v>3.25</v>
-      </c>
-      <c r="W32" t="str">
+        <v>0.65</v>
+      </c>
+      <c r="W32" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="6">
         <v>0.65300000000000002</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
-      <c r="M33">
+      <c r="L33" s="6">
+        <v>1</v>
+      </c>
+      <c r="M33" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O33">
+      <c r="N33" s="6">
+        <v>10</v>
+      </c>
+      <c r="O33" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="P33" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S33">
+      <c r="S33" s="6">
         <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="T33" t="str">
+        <v>0</v>
+      </c>
+      <c r="T33" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V33">
+      <c r="V33" s="6">
         <f t="shared" si="2"/>
-        <v>3.8</v>
-      </c>
-      <c r="W33" t="str">
+        <v>0</v>
+      </c>
+      <c r="W33" s="6" t="str">
         <f t="shared" si="3"/>
         <v>DIGIKEY</v>
       </c>
@@ -4360,7 +4376,7 @@
       <c r="F34" t="s">
         <v>227</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="3">
         <v>0.15</v>
       </c>
       <c r="H34">
@@ -4378,7 +4394,7 @@
       </c>
       <c r="O34">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="P34">
         <f t="shared" si="6"/>
@@ -4394,7 +4410,7 @@
       </c>
       <c r="S34">
         <f t="shared" si="0"/>
-        <v>0.57499999999999996</v>
+        <v>0.75</v>
       </c>
       <c r="T34">
         <f t="shared" si="1"/>
@@ -4409,73 +4425,73 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="35" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="8">
         <v>0.15</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="6">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L35">
-        <v>1</v>
-      </c>
-      <c r="M35">
+      <c r="L35" s="6">
+        <v>1</v>
+      </c>
+      <c r="M35" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O35">
+      <c r="O35" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="P35" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R35">
+      <c r="R35" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S35">
+      <c r="S35" s="6">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="T35">
+        <v>0.15</v>
+      </c>
+      <c r="T35" s="6">
         <f t="shared" si="1"/>
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="V35">
+      <c r="V35" s="6">
         <f t="shared" si="9"/>
-        <v>0.75</v>
-      </c>
-      <c r="W35" t="str">
+        <v>0.15</v>
+      </c>
+      <c r="W35" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
@@ -4499,7 +4515,7 @@
       <c r="F36" t="s">
         <v>226</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="3">
         <v>0.15</v>
       </c>
       <c r="H36">
@@ -4517,7 +4533,7 @@
       </c>
       <c r="O36">
         <f t="shared" si="5"/>
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="P36">
         <f t="shared" si="6"/>
@@ -4533,7 +4549,7 @@
       </c>
       <c r="S36">
         <f t="shared" si="0"/>
-        <v>1.0349999999999999</v>
+        <v>1.3499999999999999</v>
       </c>
       <c r="T36">
         <f t="shared" si="1"/>
@@ -4548,67 +4564,67 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="8">
         <v>0.15</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="6">
         <v>1E-3</v>
       </c>
-      <c r="L37">
-        <v>1</v>
-      </c>
-      <c r="M37">
+      <c r="L37" s="6">
+        <v>1</v>
+      </c>
+      <c r="M37" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="P37" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q37">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R37">
+      <c r="R37" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S37">
+      <c r="S37" s="6">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="T37" t="str">
+        <v>0.15</v>
+      </c>
+      <c r="T37" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V37">
+      <c r="V37" s="6">
         <f t="shared" si="9"/>
-        <v>0.75</v>
-      </c>
-      <c r="W37" t="str">
+        <v>0.15</v>
+      </c>
+      <c r="W37" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
@@ -4632,7 +4648,7 @@
       <c r="F38" t="s">
         <v>224</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="3">
         <v>0.15</v>
       </c>
       <c r="H38">
@@ -4650,7 +4666,7 @@
       </c>
       <c r="O38">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P38">
         <f t="shared" si="6"/>
@@ -4666,7 +4682,7 @@
       </c>
       <c r="S38">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="T38">
         <f t="shared" si="1"/>
@@ -4681,262 +4697,262 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="39" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="8">
         <v>0.15</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="6">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="L39">
-        <v>1</v>
-      </c>
-      <c r="M39">
+      <c r="L39" s="6">
+        <v>1</v>
+      </c>
+      <c r="M39" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="P39" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R39">
+      <c r="R39" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S39">
+      <c r="S39" s="6">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="T39" t="str">
+        <v>0.15</v>
+      </c>
+      <c r="T39" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V39">
+      <c r="V39" s="6">
         <f t="shared" si="9"/>
-        <v>0.75</v>
-      </c>
-      <c r="W39" t="str">
+        <v>0.15</v>
+      </c>
+      <c r="W39" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="8">
         <v>0.15</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="6">
         <v>1E-3</v>
       </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-      <c r="M40">
+      <c r="L40" s="6">
+        <v>1</v>
+      </c>
+      <c r="M40" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="P40" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R40">
+      <c r="R40" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S40">
+      <c r="S40" s="6">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="T40" t="str">
+        <v>0.15</v>
+      </c>
+      <c r="T40" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V40">
+      <c r="V40" s="6">
         <f t="shared" si="9"/>
-        <v>0.75</v>
-      </c>
-      <c r="W40" t="str">
+        <v>0.15</v>
+      </c>
+      <c r="W40" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="6">
         <v>0.70499999999999996</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="6">
         <v>6.9500000000000006E-2</v>
       </c>
-      <c r="L41">
-        <v>1</v>
-      </c>
-      <c r="M41">
+      <c r="L41" s="6">
+        <v>1</v>
+      </c>
+      <c r="M41" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="P41" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R41">
+      <c r="R41" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S41">
+      <c r="S41" s="6">
         <f t="shared" si="0"/>
-        <v>6.05</v>
-      </c>
-      <c r="T41" t="str">
+        <v>1.21</v>
+      </c>
+      <c r="T41" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V41">
+      <c r="V41" s="6">
         <f t="shared" si="9"/>
-        <v>6.05</v>
-      </c>
-      <c r="W41" t="str">
+        <v>1.21</v>
+      </c>
+      <c r="W41" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="8">
         <v>2</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="8">
         <v>0.15</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="6">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="6">
         <v>2</v>
       </c>
-      <c r="M42">
+      <c r="M42" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="6">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="P42">
+        <v>2</v>
+      </c>
+      <c r="P42" s="6">
         <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="Q42">
+        <v>2</v>
+      </c>
+      <c r="Q42" s="6">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="R42">
+      <c r="R42" s="6">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="S42">
+      <c r="S42" s="6">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="T42" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="T42" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V42">
+      <c r="V42" s="6">
         <f t="shared" si="9"/>
-        <v>1.5</v>
-      </c>
-      <c r="W42" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="W42" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
@@ -4960,7 +4976,7 @@
       <c r="F43" t="s">
         <v>219</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="3">
         <v>0.15</v>
       </c>
       <c r="H43">
@@ -4978,7 +4994,7 @@
       </c>
       <c r="O43">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="P43">
         <f t="shared" si="6"/>
@@ -4994,7 +5010,7 @@
       </c>
       <c r="S43">
         <f t="shared" si="0"/>
-        <v>0.45999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="T43">
         <f t="shared" si="1"/>
@@ -5028,7 +5044,7 @@
       <c r="F44" t="s">
         <v>218</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G44" s="3">
         <v>0.15</v>
       </c>
       <c r="H44">
@@ -5046,7 +5062,7 @@
       </c>
       <c r="O44">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P44">
         <f t="shared" si="6"/>
@@ -5062,7 +5078,7 @@
       </c>
       <c r="S44">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="T44">
         <f t="shared" si="1"/>
@@ -5096,7 +5112,7 @@
       <c r="F45" t="s">
         <v>217</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="3">
         <v>0.15</v>
       </c>
       <c r="H45">
@@ -5114,7 +5130,7 @@
       </c>
       <c r="O45">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P45">
         <f t="shared" si="6"/>
@@ -5130,7 +5146,7 @@
       </c>
       <c r="S45">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="T45">
         <f t="shared" si="1"/>
@@ -5164,7 +5180,7 @@
       <c r="F46" t="s">
         <v>326</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="3">
         <v>0.15</v>
       </c>
       <c r="H46">
@@ -5182,7 +5198,7 @@
       </c>
       <c r="O46">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P46">
         <f t="shared" si="6"/>
@@ -5198,7 +5214,7 @@
       </c>
       <c r="S46">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.15</v>
       </c>
       <c r="T46">
         <f t="shared" si="1"/>
@@ -5232,7 +5248,7 @@
       <c r="F47" t="s">
         <v>216</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="3">
         <v>0.15</v>
       </c>
       <c r="H47">
@@ -5250,7 +5266,7 @@
       </c>
       <c r="O47">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P47">
         <f t="shared" si="6"/>
@@ -5266,7 +5282,7 @@
       </c>
       <c r="S47">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="T47">
         <f t="shared" si="1"/>
@@ -5281,232 +5297,232 @@
         <v>JLC</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="48" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="8">
         <v>0.15</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="6">
         <v>1E-3</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="6">
         <v>2</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="O48">
+      <c r="O48" s="6">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="P48">
+        <v>2</v>
+      </c>
+      <c r="P48" s="6">
         <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="Q48">
+        <v>2</v>
+      </c>
+      <c r="Q48" s="6">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="R48">
+      <c r="R48" s="6">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="S48">
+      <c r="S48" s="6">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="T48">
+        <v>0.3</v>
+      </c>
+      <c r="T48" s="6">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
-      <c r="V48">
+      <c r="V48" s="6">
         <f t="shared" si="9"/>
-        <v>1.5</v>
-      </c>
-      <c r="W48" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="W48" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="G49" s="5">
+      <c r="G49" s="8">
         <v>0.15</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="6">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L49">
-        <v>1</v>
-      </c>
-      <c r="M49">
+      <c r="L49" s="6">
+        <v>1</v>
+      </c>
+      <c r="M49" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O49">
+      <c r="O49" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="P49" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q49">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R49">
+      <c r="R49" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S49">
+      <c r="S49" s="6">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="T49">
+        <v>0.15</v>
+      </c>
+      <c r="T49" s="6">
         <f t="shared" si="1"/>
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="V49">
+      <c r="V49" s="6">
         <f t="shared" si="9"/>
-        <v>0.75</v>
-      </c>
-      <c r="W49" t="str">
+        <v>0.15</v>
+      </c>
+      <c r="W49" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="Z49" t="s">
+      <c r="Z49" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="AA49" s="3">
-        <v>62.04</v>
-      </c>
-      <c r="AD49" s="3"/>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="AA49" s="7">
+        <v>41.1</v>
+      </c>
+      <c r="AD49" s="7"/>
+    </row>
+    <row r="50" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="G50" s="5">
+      <c r="G50" s="8">
         <v>0.15</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="6">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="6">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="6">
         <v>2</v>
       </c>
-      <c r="M50">
+      <c r="M50" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="O50">
+      <c r="O50" s="6">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="P50">
+        <v>2</v>
+      </c>
+      <c r="P50" s="6">
         <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="Q50">
+        <v>2</v>
+      </c>
+      <c r="Q50" s="6">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="R50">
+      <c r="R50" s="6">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="S50">
+      <c r="S50" s="6">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="T50">
+        <v>0.3</v>
+      </c>
+      <c r="T50" s="6">
         <f t="shared" si="1"/>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="V50">
+      <c r="V50" s="6">
         <f t="shared" si="9"/>
-        <v>1.5</v>
-      </c>
-      <c r="W50" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="W50" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="Z50" t="s">
+      <c r="Z50" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="AA50" s="3">
-        <v>33.700000000000003</v>
-      </c>
-      <c r="AD50" s="3"/>
+      <c r="AA50" s="7">
+        <v>10.73</v>
+      </c>
+      <c r="AD50" s="7"/>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -5527,7 +5543,7 @@
       <c r="F51" t="s">
         <v>213</v>
       </c>
-      <c r="G51" s="5">
+      <c r="G51" s="3">
         <v>0.15</v>
       </c>
       <c r="H51">
@@ -5545,7 +5561,7 @@
       </c>
       <c r="O51">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P51">
         <f t="shared" si="6"/>
@@ -5561,7 +5577,7 @@
       </c>
       <c r="S51">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.15</v>
       </c>
       <c r="T51">
         <f t="shared" si="1"/>
@@ -5578,10 +5594,10 @@
       <c r="Z51" t="s">
         <v>270</v>
       </c>
-      <c r="AA51" s="3">
-        <v>10.59</v>
-      </c>
-      <c r="AD51" s="3"/>
+      <c r="AA51" s="2">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AD51" s="2"/>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -5602,7 +5618,7 @@
       <c r="F52" t="s">
         <v>212</v>
       </c>
-      <c r="G52" s="5">
+      <c r="G52" s="3">
         <v>0.15</v>
       </c>
       <c r="H52">
@@ -5620,7 +5636,7 @@
       </c>
       <c r="O52">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P52">
         <f t="shared" si="6"/>
@@ -5636,7 +5652,7 @@
       </c>
       <c r="S52">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="T52">
         <f t="shared" si="1"/>
@@ -5653,11 +5669,11 @@
       <c r="Z52" t="s">
         <v>271</v>
       </c>
-      <c r="AA52" s="3">
-        <v>81.3</v>
-      </c>
-      <c r="AB52" s="2"/>
-      <c r="AD52" s="3"/>
+      <c r="AA52" s="2">
+        <v>4.59</v>
+      </c>
+      <c r="AB52" s="1"/>
+      <c r="AD52" s="2"/>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -5678,7 +5694,7 @@
       <c r="F53" t="s">
         <v>211</v>
       </c>
-      <c r="G53" s="5">
+      <c r="G53" s="3">
         <v>0.15</v>
       </c>
       <c r="H53">
@@ -5696,7 +5712,7 @@
       </c>
       <c r="O53">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="P53">
         <f t="shared" si="6"/>
@@ -5712,7 +5728,7 @@
       </c>
       <c r="S53">
         <f t="shared" si="0"/>
-        <v>0.34499999999999997</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="T53">
         <f t="shared" si="1"/>
@@ -5729,158 +5745,150 @@
       <c r="Z53" t="s">
         <v>272</v>
       </c>
-      <c r="AA53" s="3">
-        <v>52.52</v>
-      </c>
-      <c r="AB53" s="6">
-        <f>W70</f>
-        <v>20.877440000000004</v>
-      </c>
-      <c r="AD53" s="3"/>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="AA53" s="2">
+        <v>3.85</v>
+      </c>
+      <c r="AB53" s="4"/>
+      <c r="AD53" s="2"/>
+    </row>
+    <row r="54" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="6">
         <v>4.0670000000000002</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L54">
+      <c r="L54" s="6">
         <v>2</v>
       </c>
-      <c r="M54">
+      <c r="M54" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="N54">
-        <v>10</v>
-      </c>
-      <c r="O54">
+      <c r="O54" s="6">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="P54">
+        <v>2</v>
+      </c>
+      <c r="P54" s="6">
         <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="Q54">
+        <v>2</v>
+      </c>
+      <c r="Q54" s="6">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="R54">
+      <c r="R54" s="6">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="S54">
+      <c r="S54" s="6">
         <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="T54" t="str">
+        <v>9.6</v>
+      </c>
+      <c r="T54" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V54">
+      <c r="V54" s="6">
         <f t="shared" si="9"/>
-        <v>48</v>
-      </c>
-      <c r="W54" t="str">
+        <v>9.6</v>
+      </c>
+      <c r="W54" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="X54" t="s">
+      <c r="X54" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="Z54" t="s">
+      <c r="Z54" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="AA54" s="3">
-        <v>6.82</v>
-      </c>
-      <c r="AD54" s="3"/>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="AA54" s="7">
+        <v>0.86</v>
+      </c>
+      <c r="AD54" s="7"/>
+    </row>
+    <row r="55" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="6">
         <v>0.83</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="L55">
-        <v>1</v>
-      </c>
-      <c r="M55">
+      <c r="L55" s="6">
+        <v>1</v>
+      </c>
+      <c r="M55" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O55">
+      <c r="O55" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P55">
+        <v>1</v>
+      </c>
+      <c r="P55" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q55">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R55">
+      <c r="R55" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S55">
+      <c r="S55" s="6">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T55" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="T55" s="6" t="str">
         <f t="shared" si="1"/>
         <v>EMPTY</v>
       </c>
-      <c r="V55">
+      <c r="V55" s="6">
         <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="W55" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="W55" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="Z55" t="s">
+      <c r="Z55" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="AA55" s="3">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="AD55" s="3"/>
+      <c r="AA55" s="7"/>
+      <c r="AD55" s="7"/>
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -5895,7 +5903,7 @@
       <c r="E56" t="s">
         <v>171</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56" s="3">
         <v>13.35</v>
       </c>
       <c r="H56">
@@ -5913,11 +5921,11 @@
       </c>
       <c r="O56">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P56">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q56">
         <f t="shared" si="7"/>
@@ -5929,7 +5937,7 @@
       </c>
       <c r="S56">
         <f t="shared" si="0"/>
-        <v>66.75</v>
+        <v>0</v>
       </c>
       <c r="T56" t="str">
         <f t="shared" si="1"/>
@@ -5937,7 +5945,7 @@
       </c>
       <c r="V56">
         <f t="shared" si="9"/>
-        <v>66.75</v>
+        <v>0</v>
       </c>
       <c r="W56" t="str">
         <f t="shared" si="10"/>
@@ -5949,10 +5957,8 @@
       <c r="Z56" t="s">
         <v>328</v>
       </c>
-      <c r="AA56" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="AD56" s="3"/>
+      <c r="AA56" s="2"/>
+      <c r="AD56" s="2"/>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -5973,7 +5979,7 @@
       <c r="F57" t="s">
         <v>210</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G57" s="3">
         <v>1.06</v>
       </c>
       <c r="H57">
@@ -5991,7 +5997,7 @@
       </c>
       <c r="O57">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P57">
         <f t="shared" si="6"/>
@@ -6007,7 +6013,7 @@
       </c>
       <c r="S57">
         <f t="shared" si="0"/>
-        <v>5.3000000000000007</v>
+        <v>1.06</v>
       </c>
       <c r="T57">
         <f t="shared" si="1"/>
@@ -6027,10 +6033,10 @@
       <c r="Z57" t="s">
         <v>275</v>
       </c>
-      <c r="AA57" s="3">
-        <v>60.96</v>
-      </c>
-      <c r="AD57" s="3"/>
+      <c r="AA57" s="2">
+        <v>34.619999999999997</v>
+      </c>
+      <c r="AD57" s="2"/>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
@@ -6094,89 +6100,88 @@
         <v>DIGIKEY</v>
       </c>
       <c r="Z58" t="s">
-        <v>276</v>
-      </c>
-      <c r="AA58" s="3">
-        <f>SUM(AA49:AA51)+AB53+SUM(AA54:AA57)</f>
-        <v>196.21744000000001</v>
-      </c>
-      <c r="AD58" s="3"/>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA58" s="2">
+        <v>-12.08</v>
+      </c>
+      <c r="AD58" s="2"/>
+    </row>
+    <row r="59" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="6">
         <v>0.45600000000000002</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="6">
         <v>0.1439</v>
       </c>
-      <c r="L59">
-        <v>1</v>
-      </c>
-      <c r="M59">
+      <c r="L59" s="6">
+        <v>1</v>
+      </c>
+      <c r="M59" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O59">
+      <c r="O59" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P59">
+        <v>1</v>
+      </c>
+      <c r="P59" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q59">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R59">
+      <c r="R59" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S59">
+      <c r="S59" s="6">
         <f t="shared" si="0"/>
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="T59">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="T59" s="6">
         <f t="shared" si="1"/>
         <v>4.7595000000000001</v>
       </c>
-      <c r="V59">
+      <c r="V59" s="6">
         <f t="shared" si="9"/>
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="W59" t="str">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="W59" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="Z59" t="s">
-        <v>277</v>
-      </c>
-      <c r="AA59" s="3">
-        <f>0.12*AA58</f>
-        <v>23.5460928</v>
-      </c>
-      <c r="AD59" s="3"/>
+      <c r="Z59" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="AA59" s="7">
+        <f>SUM(AA49:AA58)</f>
+        <v>85.679999999999993</v>
+      </c>
+      <c r="AD59" s="7"/>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
@@ -6218,11 +6223,11 @@
       </c>
       <c r="O60">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P60">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q60">
         <f t="shared" si="7"/>
@@ -6234,7 +6239,7 @@
       </c>
       <c r="S60">
         <f t="shared" si="0"/>
-        <v>74.7</v>
+        <v>0</v>
       </c>
       <c r="T60">
         <f t="shared" si="1"/>
@@ -6242,7 +6247,7 @@
       </c>
       <c r="V60">
         <f t="shared" si="9"/>
-        <v>74.7</v>
+        <v>0</v>
       </c>
       <c r="W60" t="str">
         <f t="shared" si="10"/>
@@ -6252,91 +6257,91 @@
         <v>332</v>
       </c>
       <c r="Z60" t="s">
-        <v>278</v>
-      </c>
-      <c r="AA60" s="3">
-        <v>17.5</v>
-      </c>
-      <c r="AD60" s="3"/>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA60" s="2">
+        <f>0.12*AA59</f>
+        <v>10.281599999999999</v>
+      </c>
+      <c r="AD60" s="2"/>
+    </row>
+    <row r="61" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="6">
         <v>2.31</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="6">
         <v>0.498</v>
       </c>
-      <c r="L61">
-        <v>1</v>
-      </c>
-      <c r="M61">
+      <c r="L61" s="6">
+        <v>1</v>
+      </c>
+      <c r="M61" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O61">
+      <c r="O61" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P61">
+        <v>1</v>
+      </c>
+      <c r="P61" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q61">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R61">
+      <c r="R61" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S61">
+      <c r="S61" s="6">
         <f t="shared" si="0"/>
-        <v>12.7</v>
-      </c>
-      <c r="T61">
+        <v>2.54</v>
+      </c>
+      <c r="T61" s="6">
         <f t="shared" si="1"/>
         <v>2.4900000000000002</v>
       </c>
-      <c r="U61" t="s">
+      <c r="U61" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="V61">
+      <c r="V61" s="6">
         <f t="shared" si="9"/>
-        <v>12.7</v>
-      </c>
-      <c r="W61" t="str">
+        <v>2.54</v>
+      </c>
+      <c r="W61" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="Z61" t="s">
-        <v>266</v>
-      </c>
-      <c r="AA61" s="3">
-        <f>SUM(AA58:AA60)</f>
-        <v>237.26353280000001</v>
-      </c>
-      <c r="AD61" s="3"/>
+      <c r="Z61" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="AA61" s="7">
+        <v>17.5</v>
+      </c>
+      <c r="AD61" s="7"/>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -6354,7 +6359,7 @@
       <c r="F62" t="s">
         <v>265</v>
       </c>
-      <c r="G62" s="5">
+      <c r="G62" s="3">
         <v>4.82</v>
       </c>
       <c r="H62">
@@ -6411,8 +6416,14 @@
       <c r="X62" t="s">
         <v>334</v>
       </c>
-      <c r="AA62" s="3"/>
-      <c r="AD62" s="3"/>
+      <c r="Z62" t="s">
+        <v>266</v>
+      </c>
+      <c r="AA62" s="2">
+        <f>SUM(AA59:AA61)</f>
+        <v>113.46159999999999</v>
+      </c>
+      <c r="AD62" s="2"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -6487,160 +6498,161 @@
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="AA63" s="3">
-        <f>AA61+X70</f>
-        <v>665.43953280000005</v>
-      </c>
-      <c r="AD63" s="3"/>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="AA63" s="2"/>
+      <c r="AD63" s="2"/>
+    </row>
+    <row r="64" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="6">
         <v>0.28699999999999998</v>
       </c>
-      <c r="I64">
+      <c r="I64" s="6">
         <v>0.1118</v>
       </c>
-      <c r="L64">
+      <c r="L64" s="6">
         <v>2</v>
       </c>
-      <c r="M64">
+      <c r="M64" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="O64">
+      <c r="O64" s="6">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="P64">
+        <v>2</v>
+      </c>
+      <c r="P64" s="6">
         <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="Q64">
+        <v>2</v>
+      </c>
+      <c r="Q64" s="6">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="R64">
+      <c r="R64" s="6">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="S64">
+      <c r="S64" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T64">
+        <v>0.6</v>
+      </c>
+      <c r="T64" s="6">
         <f t="shared" si="1"/>
         <v>5.1579999999999995</v>
       </c>
-      <c r="V64">
+      <c r="V64" s="6">
         <f t="shared" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="W64" t="str">
+        <v>0.6</v>
+      </c>
+      <c r="W64" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
-      <c r="Z64" t="s">
-        <v>279</v>
-      </c>
-      <c r="AA64" s="3">
-        <f>AA63/10</f>
-        <v>66.543953280000011</v>
-      </c>
-      <c r="AD64" s="3"/>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="AA64" s="7">
+        <f>AA62+X70</f>
+        <v>140.0728</v>
+      </c>
+      <c r="AD64" s="7"/>
+    </row>
+    <row r="65" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="H65">
+      <c r="H65" s="6">
         <v>0.70499999999999996</v>
       </c>
-      <c r="I65">
+      <c r="I65" s="6">
         <v>0.76160000000000005</v>
       </c>
-      <c r="L65">
-        <v>1</v>
-      </c>
-      <c r="M65">
+      <c r="L65" s="6">
+        <v>1</v>
+      </c>
+      <c r="M65" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O65">
+      <c r="O65" s="6">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P65">
+        <v>1</v>
+      </c>
+      <c r="P65" s="6">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Q65">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="6">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R65">
+      <c r="R65" s="6">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S65">
+      <c r="S65" s="6">
         <f t="shared" si="0"/>
-        <v>4.25</v>
-      </c>
-      <c r="T65">
+        <v>0.85</v>
+      </c>
+      <c r="T65" s="6">
         <f t="shared" si="1"/>
         <v>7.8480000000000008</v>
       </c>
-      <c r="U65" t="s">
+      <c r="U65" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="V65">
+      <c r="V65" s="6">
         <f t="shared" si="9"/>
-        <v>4.25</v>
-      </c>
-      <c r="W65" t="str">
+        <v>0.85</v>
+      </c>
+      <c r="W65" s="6" t="str">
         <f t="shared" si="10"/>
         <v>DIGIKEY</v>
       </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z65" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="AA65" s="7">
+        <f>AA64/10</f>
+        <v>14.00728</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>199</v>
       </c>
@@ -6715,105 +6727,105 @@
       </c>
       <c r="X66">
         <f>COUNTIF(W2:W66,"DIGIKEY")-5</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="6">
         <v>0.45</v>
       </c>
-      <c r="H67">
+      <c r="H67" s="6">
         <v>0.312</v>
       </c>
-      <c r="I67">
+      <c r="I67" s="6">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="L67">
+      <c r="L67" s="6">
         <v>3</v>
       </c>
-      <c r="M67">
+      <c r="M67" s="6">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="O67">
-        <f t="shared" ref="O67" si="14">M67*5</f>
-        <v>15</v>
-      </c>
-      <c r="P67">
+      <c r="O67" s="6">
+        <f t="shared" ref="O67" si="14">IF(M67-N67&lt;0,0, M67-N67)</f>
+        <v>3</v>
+      </c>
+      <c r="P67" s="6">
         <f t="shared" ref="P67" si="15">IF(W67="DIGIKEY",O67,0)</f>
-        <v>15</v>
-      </c>
-      <c r="Q67">
+        <v>3</v>
+      </c>
+      <c r="Q67" s="6">
         <f t="shared" ref="Q67" si="16">M67*8</f>
         <v>24</v>
       </c>
-      <c r="R67">
+      <c r="R67" s="6">
         <f t="shared" ref="R67" si="17">M67*5</f>
         <v>15</v>
       </c>
-      <c r="S67">
+      <c r="S67" s="6">
         <f>IF(O67&gt;10,H67*O67,G67*O67)</f>
-        <v>4.68</v>
-      </c>
-      <c r="T67">
+        <v>1.35</v>
+      </c>
+      <c r="T67" s="6">
         <f>IF(ISBLANK(D67),"EMPTY",(I67*R67+IF(D67="yes",4.04,0)))</f>
         <v>5.2774999999999999</v>
       </c>
-      <c r="V67">
+      <c r="V67" s="6">
         <f t="shared" ref="V67" si="18">IF(T67="EMPTY",S67,IF(J67="Bottom",S67,IF(U67="DIGIKEY",S67,IF(U67="JLC",T67,IF(T67&lt;S67+0.2,T67,S67)))))</f>
-        <v>4.68</v>
-      </c>
-      <c r="W67" t="str">
+        <v>1.35</v>
+      </c>
+      <c r="W67" s="6" t="str">
         <f t="shared" ref="W67" si="19">IF(T67="EMPTY","DIGIKEY",IF(J67="Bottom","DIGIKEY",IF(U67="DIGIKEY",U67,IF(U67="JLC",U67,IF(T67&lt;S67+0.2,"JLC","DIGIKEY")))))</f>
         <v>DIGIKEY</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="W69">
         <f>COUNTIF(W2:W66,"JLC")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="X69">
         <f>SUMIF(W2:W66,"DIGIKEY",Q2:Q66)</f>
-        <v>280</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="T70" t="s">
         <v>266</v>
       </c>
       <c r="V70">
         <f>SUM(V2:V66)</f>
-        <v>398.61049999999994</v>
-      </c>
-      <c r="W70" s="7">
+        <v>40.083500000000008</v>
+      </c>
+      <c r="W70" s="5">
         <f>SUMIF(W2:W66,"JLC",V2:V66)*1.28</f>
-        <v>20.877440000000004</v>
+        <v>20.894080000000002</v>
       </c>
       <c r="X70">
         <f>SUMIF(W2:W66,"DIGIKEY",V2:V66)*1.12</f>
-        <v>428.17600000000004</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+        <v>26.611200000000004</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.3">
       <c r="T71" t="s">
         <v>267</v>
       </c>
@@ -6824,24 +6836,24 @@
         <v>327</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="W73" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.3">
       <c r="V74">
         <f>V60+V56+V31++V4</f>
-        <v>229.04999999999998</v>
+        <v>0</v>
       </c>
       <c r="X74" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.3">
       <c r="X75">
         <f>X69/8</f>
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>